<commit_message>
Updated Excel File & Added File -> Delete Node in Linked List
</commit_message>
<xml_diff>
--- a/DSA Tracker.xlsx
+++ b/DSA Tracker.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2774" uniqueCount="1070">
   <si>
     <t>Date</t>
   </si>
@@ -4536,8 +4536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="C2" s="77">
         <f>COUNTIF(F10:F1005,"=1")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="128"/>
       <c r="E2" s="128"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="C7" s="78">
         <f>SUM(G10:G1008)</f>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E7" s="128"/>
       <c r="F7" s="128"/>
@@ -5380,10 +5380,16 @@
       <c r="C43" s="82" t="s">
         <v>1069</v>
       </c>
-      <c r="D43" s="80"/>
+      <c r="D43" s="80" t="s">
+        <v>105</v>
+      </c>
       <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="75"/>
+      <c r="F43" s="80">
+        <v>1</v>
+      </c>
+      <c r="G43" s="75">
+        <v>1</v>
+      </c>
       <c r="H43" s="83"/>
       <c r="I43" s="85"/>
     </row>

</xml_diff>